<commit_message>
fix(pipelining): fix LoadStore instructions with WB #2
</commit_message>
<xml_diff>
--- a/programs/fpu-maclaurin-program-sin-pi-over-2.xlsx
+++ b/programs/fpu-maclaurin-program-sin-pi-over-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AD58EF-33B5-433F-A1FC-A71B6AECA139}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFD3593-7AC9-4A25-A9C8-FC3E5BA24245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
   <si>
     <t>Hex</t>
   </si>
@@ -303,10 +303,25 @@
     <t>Data memory</t>
   </si>
   <si>
-    <t>MOV R0 = 0 ROR #0</t>
-  </si>
-  <si>
     <t>3BF5</t>
+  </si>
+  <si>
+    <t>MOV R0 = 0 ROR #12</t>
+  </si>
+  <si>
+    <t>0x012</t>
+  </si>
+  <si>
+    <t>0x013</t>
+  </si>
+  <si>
+    <t>0x014</t>
+  </si>
+  <si>
+    <t>0x015</t>
+  </si>
+  <si>
+    <t>0x016</t>
   </si>
 </sst>
 </file>
@@ -703,8 +718,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,7 +1025,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -1046,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="3">
         <v>0</v>
@@ -1055,14 +1070,14 @@
         <v>0</v>
       </c>
       <c r="Q9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="3">
         <v>0</v>
       </c>
       <c r="S9" s="3" t="str">
         <f>DEC2HEX(C9*2^15 + D9*2^14 + E9*2^13 + F9*2^12 + G9*2^11 + H9*2^10 + I9*2^9 + J9*2^8 + K9*2^7 + L9*2^6 + M9*2^5 + N9*2^4 + O9 * 2 ^ 3 + P9  * 2^2 + Q9 * 2 + R9)</f>
-        <v>C200</v>
+        <v>C212</v>
       </c>
       <c r="T9" t="s">
         <v>55</v>
@@ -2218,7 +2233,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>50</v>
@@ -2278,7 +2293,7 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
         <v>51</v>
@@ -2338,7 +2353,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
         <v>66</v>
@@ -2349,7 +2364,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
         <v>52</v>
@@ -2409,19 +2424,19 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
         <v>65</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T32" t="s">
         <v>67</v>
       </c>
       <c r="U32" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V32">
         <v>0.99462890625</v>
@@ -2513,6 +2528,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="K7:P7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A27:S27"/>
     <mergeCell ref="D3:F3"/>
@@ -2529,14 +2552,6 @@
     <mergeCell ref="I6:R6"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="K7:P7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="M5:P5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>